<commit_message>
description updated, added recommendation column
</commit_message>
<xml_diff>
--- a/Autoimmune_Disorder_Description.xlsx
+++ b/Autoimmune_Disorder_Description.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marszu/Documents/Project_test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marszu/Documents/ISA/jdszr16-random-forest-rangers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB19229-61F3-C943-B25D-CD597D7C12B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF417889-6117-F04B-9A85-72CC4BB331E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2660" yWindow="500" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$117</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$117</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="487">
   <si>
     <t>Linear IgA disease</t>
   </si>
@@ -1463,13 +1463,46 @@
   </si>
   <si>
     <t>Immune System Diseases</t>
+  </si>
+  <si>
+    <t>Consult dermatologist</t>
+  </si>
+  <si>
+    <t>Consult rheumatologist</t>
+  </si>
+  <si>
+    <t>Endocrinologist visit</t>
+  </si>
+  <si>
+    <t>See neurologist</t>
+  </si>
+  <si>
+    <t>Seek specialist advice</t>
+  </si>
+  <si>
+    <t>Consult vascular specialist</t>
+  </si>
+  <si>
+    <t>Check with nephrologist</t>
+  </si>
+  <si>
+    <t>Consult gastroenterologist</t>
+  </si>
+  <si>
+    <t>Visit immunologist</t>
+  </si>
+  <si>
+    <t>Recommendation</t>
+  </si>
+  <si>
+    <t>Visit to a specialist is not required</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1493,6 +1526,13 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1536,13 +1576,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1847,10 +1888,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F117"/>
+  <dimension ref="A1:G117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1861,9 +1902,10 @@
     <col min="4" max="4" width="53.83203125" customWidth="1"/>
     <col min="5" max="5" width="196.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="138.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>466</v>
       </c>
@@ -1882,8 +1924,11 @@
       <c r="F1" s="3" t="s">
         <v>464</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="4" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1902,8 +1947,11 @@
       <c r="F2" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1922,8 +1970,11 @@
       <c r="F3" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1942,8 +1993,11 @@
       <c r="F4" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1962,8 +2016,11 @@
       <c r="F5" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1982,8 +2039,11 @@
       <c r="F6" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2002,8 +2062,11 @@
       <c r="F7" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2022,8 +2085,11 @@
       <c r="F8" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2042,8 +2108,11 @@
       <c r="F9" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2062,8 +2131,11 @@
       <c r="F10" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2082,8 +2154,11 @@
       <c r="F11" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2102,8 +2177,11 @@
       <c r="F12" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2122,8 +2200,11 @@
       <c r="F13" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2142,8 +2223,11 @@
       <c r="F14" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2162,8 +2246,11 @@
       <c r="F15" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2182,8 +2269,11 @@
       <c r="F16" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2202,8 +2292,11 @@
       <c r="F17" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2222,8 +2315,11 @@
       <c r="F18" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2242,8 +2338,11 @@
       <c r="F19" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2262,8 +2361,11 @@
       <c r="F20" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2282,8 +2384,11 @@
       <c r="F21" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2302,8 +2407,11 @@
       <c r="F22" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2322,8 +2430,11 @@
       <c r="F23" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2342,8 +2453,11 @@
       <c r="F24" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2362,8 +2476,11 @@
       <c r="F25" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2382,8 +2499,11 @@
       <c r="F26" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2402,8 +2522,11 @@
       <c r="F27" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2422,8 +2545,11 @@
       <c r="F28" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2442,8 +2568,11 @@
       <c r="F29" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2462,8 +2591,11 @@
       <c r="F30" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2482,8 +2614,11 @@
       <c r="F31" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2502,8 +2637,11 @@
       <c r="F32" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G32" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2522,8 +2660,11 @@
       <c r="F33" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G33" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2542,8 +2683,11 @@
       <c r="F34" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G34" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2562,8 +2706,11 @@
       <c r="F35" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G35" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2582,8 +2729,11 @@
       <c r="F36" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G36" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2602,8 +2752,11 @@
       <c r="F37" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G37" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2622,8 +2775,11 @@
       <c r="F38" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G38" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2642,8 +2798,11 @@
       <c r="F39" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G39" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2662,8 +2821,11 @@
       <c r="F40" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G40" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2682,8 +2844,11 @@
       <c r="F41" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G41" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2702,8 +2867,11 @@
       <c r="F42" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G42" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2722,8 +2890,11 @@
       <c r="F43" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G43" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2742,8 +2913,11 @@
       <c r="F44" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G44" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2762,8 +2936,11 @@
       <c r="F45" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G45" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2782,8 +2959,11 @@
       <c r="F46" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G46" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2802,8 +2982,11 @@
       <c r="F47" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G47" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2822,8 +3005,11 @@
       <c r="F48" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G48" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2842,8 +3028,11 @@
       <c r="F49" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G49" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2862,8 +3051,11 @@
       <c r="F50" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G50" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2882,8 +3074,11 @@
       <c r="F51" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G51" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2902,8 +3097,11 @@
       <c r="F52" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G52" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2922,8 +3120,11 @@
       <c r="F53" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G53" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2942,8 +3143,11 @@
       <c r="F54" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G54" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2962,8 +3166,11 @@
       <c r="F55" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G55" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2982,8 +3189,11 @@
       <c r="F56" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G56" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -3002,8 +3212,11 @@
       <c r="F57" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G57" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3022,8 +3235,11 @@
       <c r="F58" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G58" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3042,8 +3258,11 @@
       <c r="F59" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G59" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3062,8 +3281,11 @@
       <c r="F60" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G60" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3082,8 +3304,11 @@
       <c r="F61" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G61" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3102,8 +3327,11 @@
       <c r="F62" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G62" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -3122,8 +3350,11 @@
       <c r="F63" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G63" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -3142,8 +3373,11 @@
       <c r="F64" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G64" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -3162,8 +3396,11 @@
       <c r="F65" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G65" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -3182,8 +3419,11 @@
       <c r="F66" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G66" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -3202,8 +3442,11 @@
       <c r="F67" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G67" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -3222,8 +3465,11 @@
       <c r="F68" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G68" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -3242,8 +3488,11 @@
       <c r="F69" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G69" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -3262,8 +3511,11 @@
       <c r="F70" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G70" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -3282,8 +3534,11 @@
       <c r="F71" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G71" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -3302,8 +3557,11 @@
       <c r="F72" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G72" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -3322,8 +3580,11 @@
       <c r="F73" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G73" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -3342,8 +3603,11 @@
       <c r="F74" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G74" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -3362,8 +3626,11 @@
       <c r="F75" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G75" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -3382,8 +3649,11 @@
       <c r="F76" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G76" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -3402,8 +3672,11 @@
       <c r="F77" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G77" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -3422,8 +3695,11 @@
       <c r="F78" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G78" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -3442,8 +3718,11 @@
       <c r="F79" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G79" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
@@ -3462,8 +3741,11 @@
       <c r="F80" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G80" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
@@ -3482,8 +3764,11 @@
       <c r="F81" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G81" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -3502,8 +3787,11 @@
       <c r="F82" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G82" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
@@ -3522,8 +3810,11 @@
       <c r="F83" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G83" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
@@ -3542,8 +3833,11 @@
       <c r="F84" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G84" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -3562,8 +3856,11 @@
       <c r="F85" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G85" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
@@ -3582,8 +3879,11 @@
       <c r="F86" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G86" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
@@ -3602,8 +3902,11 @@
       <c r="F87" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G87" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
@@ -3622,8 +3925,11 @@
       <c r="F88" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G88" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
@@ -3642,8 +3948,11 @@
       <c r="F89" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G89" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
@@ -3662,8 +3971,11 @@
       <c r="F90" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G90" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
@@ -3682,8 +3994,11 @@
       <c r="F91" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G91" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
@@ -3702,8 +4017,11 @@
       <c r="F92" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G92" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
@@ -3722,8 +4040,11 @@
       <c r="F93" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G93" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
@@ -3742,8 +4063,11 @@
       <c r="F94" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G94" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
@@ -3762,8 +4086,11 @@
       <c r="F95" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G95" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
       </c>
@@ -3782,8 +4109,11 @@
       <c r="F96" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G96" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>96</v>
       </c>
@@ -3802,8 +4132,11 @@
       <c r="F97" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G97" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>97</v>
       </c>
@@ -3822,8 +4155,11 @@
       <c r="F98" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G98" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>98</v>
       </c>
@@ -3842,8 +4178,11 @@
       <c r="F99" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G99" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>99</v>
       </c>
@@ -3862,8 +4201,11 @@
       <c r="F100" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G100" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>100</v>
       </c>
@@ -3882,8 +4224,11 @@
       <c r="F101" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G101" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>101</v>
       </c>
@@ -3902,8 +4247,11 @@
       <c r="F102" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G102" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>102</v>
       </c>
@@ -3922,8 +4270,11 @@
       <c r="F103" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G103" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>103</v>
       </c>
@@ -3942,8 +4293,11 @@
       <c r="F104" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G104" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>104</v>
       </c>
@@ -3962,8 +4316,11 @@
       <c r="F105" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G105" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>105</v>
       </c>
@@ -3982,8 +4339,11 @@
       <c r="F106" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G106" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>106</v>
       </c>
@@ -4002,8 +4362,11 @@
       <c r="F107" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G107" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>107</v>
       </c>
@@ -4022,8 +4385,11 @@
       <c r="F108" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G108" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>108</v>
       </c>
@@ -4042,8 +4408,11 @@
       <c r="F109" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G109" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>109</v>
       </c>
@@ -4062,8 +4431,11 @@
       <c r="F110" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G110" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>110</v>
       </c>
@@ -4082,8 +4454,11 @@
       <c r="F111" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G111" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>111</v>
       </c>
@@ -4102,8 +4477,11 @@
       <c r="F112" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G112" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>112</v>
       </c>
@@ -4122,8 +4500,11 @@
       <c r="F113" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G113" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>113</v>
       </c>
@@ -4142,8 +4523,11 @@
       <c r="F114" t="s">
         <v>457</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G114" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>114</v>
       </c>
@@ -4162,8 +4546,11 @@
       <c r="F115" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G115" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>115</v>
       </c>
@@ -4182,8 +4569,11 @@
       <c r="F116" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G116" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>116</v>
       </c>
@@ -4202,9 +4592,12 @@
       <c r="F117" t="s">
         <v>460</v>
       </c>
+      <c r="G117" t="s">
+        <v>486</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F117" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:G117" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>